<commit_message>
Ver.5 Prep for second print
</commit_message>
<xml_diff>
--- a/MC4BOM.xlsx
+++ b/MC4BOM.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msurv\Documents\EAGLE\projects\Benson Motor Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msurv\Documents\EAGLE\projects\Motor_Controller_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014283D1-1B2D-4AD0-8472-F3D1748E9D3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{750B0094-484B-4F69-820A-EB1A33976965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="450" windowWidth="24090" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="9585" windowWidth="24090" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MC4BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="231">
   <si>
     <t>Part</t>
   </si>
@@ -707,6 +708,12 @@
   </si>
   <si>
     <t>2725-LS03-13B05R3-ND</t>
+  </si>
+  <si>
+    <t>C921U222MVVDBA7317</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/C921U222MVVDBA7317/3645235</t>
   </si>
 </sst>
 </file>
@@ -716,7 +723,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,6 +890,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1071,7 +1084,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1186,6 +1199,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1233,7 +1255,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1256,6 +1278,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1305,128 +1330,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1437,26 +1341,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K51" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="A1:K51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Device" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="DESCRIPTION2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="HEIGHT" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="MANUFACTURER_NAME" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Price" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="MANUFACTURER_PART_NUMBER" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="URL" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1756,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,7 +2091,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -2230,7 +2114,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2251,7 +2135,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -2280,7 +2164,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2303,13 +2187,16 @@
         <v>0.46</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2338,7 +2225,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -2367,7 +2254,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -2396,7 +2283,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -2425,7 +2312,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -2446,7 +2333,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>84</v>
       </c>
@@ -2469,7 +2356,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -2492,7 +2379,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -2521,7 +2408,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -2554,7 +2441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>100</v>
       </c>
@@ -2575,7 +2462,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>103</v>
       </c>
@@ -2604,7 +2491,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -3152,6 +3039,9 @@
       <c r="J54" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K20:M20"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K48" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -3168,28 +3058,24 @@
     <hyperlink ref="K9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="K11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="K19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="K20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="K21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="K22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="K23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="K24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="K28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="K29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="K31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="K32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="K35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K36" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="K37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="K39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="K41" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="K44" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="K50" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="K51" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="K21" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="K22" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="K23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="K24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="K28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="K29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="K31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="K32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="K35" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="K36" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="K37" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="K39" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="K41" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="K44" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="K50" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="K51" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
-  <tableParts count="1">
-    <tablePart r:id="rId34"/>
-  </tableParts>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ver.5 All files added
</commit_message>
<xml_diff>
--- a/MC4BOM.xlsx
+++ b/MC4BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msurv\Documents\EAGLE\projects\Motor_Controller_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{750B0094-484B-4F69-820A-EB1A33976965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C1C6D-5112-474B-A8F9-B369EE89BB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="9585" windowWidth="24090" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3285" windowWidth="19275" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MC4BOM" sheetId="1" r:id="rId1"/>
@@ -1646,20 +1646,20 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" customWidth="1"/>
+    <col min="10" max="10" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -2022,7 +2022,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2045,7 +2045,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -2068,7 +2068,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -2114,7 +2114,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>84</v>
       </c>
@@ -2356,7 +2356,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -2379,7 +2379,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>100</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>103</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>115</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>116</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>120</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>125</v>
       </c>
@@ -2684,7 +2684,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>128</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>133</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>137</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>142</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
@@ -2819,7 +2819,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>149</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>153</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>154</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>156</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="J47" s="12"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>157</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>161</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>162</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>165</v>
       </c>
@@ -3031,11 +3031,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I53" s="11"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J54" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start routing on new board with updated components v5.1
</commit_message>
<xml_diff>
--- a/MC4BOM.xlsx
+++ b/MC4BOM.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msurv\Documents\EAGLE\projects\Motor_Controller_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C1C6D-5112-474B-A8F9-B369EE89BB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081C475E-7CEA-4011-B70C-9AD12B3AF007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3285" windowWidth="19275" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="885" windowWidth="19275" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MC4BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1642,24 +1641,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" customWidth="1"/>
-    <col min="10" max="10" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1891,7 +1890,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1978,7 +1977,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -2001,7 +2000,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -2022,7 +2021,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2045,7 +2044,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -2068,7 +2067,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2091,7 +2090,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -2114,7 +2113,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -2135,7 +2134,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2225,7 +2224,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -2312,7 +2311,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -2333,7 +2332,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>84</v>
       </c>
@@ -2356,7 +2355,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -2379,7 +2378,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>100</v>
       </c>
@@ -2462,7 +2461,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>103</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>115</v>
       </c>
@@ -2578,7 +2577,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>116</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>120</v>
       </c>
@@ -2634,7 +2633,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>125</v>
       </c>
@@ -2684,7 +2683,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>128</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>133</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>137</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>142</v>
       </c>
@@ -2796,7 +2795,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
@@ -2819,7 +2818,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>149</v>
       </c>
@@ -2848,7 +2847,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>153</v>
       </c>
@@ -2871,7 +2870,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>154</v>
       </c>
@@ -2894,7 +2893,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>156</v>
       </c>
@@ -2917,7 +2916,7 @@
       <c r="J47" s="12"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>157</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>161</v>
       </c>
@@ -2973,7 +2972,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>162</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>165</v>
       </c>
@@ -3031,11 +3030,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I53" s="11"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J54" s="13"/>
     </row>
   </sheetData>

</xml_diff>